<commit_message>
Site updated: 2021-06-06 01:41:40
</commit_message>
<xml_diff>
--- a/mqpj/母亲费用.xlsx
+++ b/mqpj/母亲费用.xlsx
@@ -1882,12 +1882,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1903,6 +1897,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2206,939 +2206,939 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H61"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
-    <col min="4" max="4" width="7.875" customWidth="1"/>
-    <col min="5" max="5" width="6.75" customWidth="1"/>
-    <col min="6" max="6" width="6.375" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="22.375" customWidth="1"/>
+    <col min="4" max="4" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="5.625" customWidth="1"/>
+    <col min="6" max="6" width="6.625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="19">
         <v>27.73</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="19">
         <v>24</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="19">
         <f t="shared" ref="D2:D8" si="0">SUM(B2:C2)</f>
         <v>51.730000000000004</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>26.73</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>24</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <f t="shared" si="0"/>
         <v>50.730000000000004</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>40.56</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <v>24</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="19">
         <f t="shared" si="0"/>
         <v>64.56</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>31.04</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>24</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="19">
         <f t="shared" si="0"/>
         <v>55.04</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>63.3</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>14</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <f t="shared" si="0"/>
         <v>77.3</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>17.399999999999999</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="19">
         <v>24</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="19">
         <f t="shared" si="0"/>
         <v>41.4</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>76.22</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>24</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="19">
         <f t="shared" si="0"/>
         <v>100.22</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="14.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="20">
         <v>212.5</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <v>212.5</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="19">
         <v>970.58</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="19">
         <v>970.58</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="19">
         <f>1000-47.18</f>
         <v>952.82</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <f>1000-47.18</f>
         <v>952.82</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="19">
         <v>10</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <v>10</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="14.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="20">
         <v>140</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19">
         <v>140</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="19">
         <v>1340</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="19">
         <v>1340</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="19">
         <v>150</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="19">
         <v>150</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="19">
         <v>150</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="19">
         <v>150</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:12" ht="14.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="20">
         <v>30</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="19">
         <v>30</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:12" ht="14.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="20">
         <v>144</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <v>144</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:12" ht="14.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="20">
         <v>20</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="19">
         <v>20</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:12" ht="14.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="21">
         <v>300</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21">
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19">
         <v>300</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="19">
         <v>1350</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19">
         <v>1350</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="19">
         <v>600</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19">
         <v>600</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="19">
         <v>539</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19">
         <v>539</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="19">
         <v>300</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19">
         <v>300</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="19">
         <v>200</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19">
         <v>200</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="19">
         <v>27</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="19">
         <v>27</v>
       </c>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="19">
         <v>9.91</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="19">
         <v>9.91</v>
       </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
       <c r="L30" s="10"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="19">
         <v>67.040000000000006</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="19">
         <v>67.040000000000006</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="19">
         <v>250</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="19">
         <v>250</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="19">
         <v>16</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21">
+      <c r="D33" s="19"/>
+      <c r="E33" s="19">
         <v>16</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="19">
         <v>1200</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21">
+      <c r="D34" s="19"/>
+      <c r="E34" s="19">
         <v>1200</v>
       </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19" t="s">
         <v>454</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="19">
         <v>860</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="19">
         <v>860</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19">
         <f>SUM(D2:D35)</f>
         <v>5634.83</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="19">
         <f>SUM(E23:E34)</f>
         <v>4205</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="19">
         <f>SUM(F14:F34)</f>
         <v>440</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="19">
         <f>SUM(D36:F36)</f>
         <v>10279.83</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="19">
         <f>G36/4</f>
         <v>2569.9575</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="19" t="s">
         <v>459</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19">
         <v>-48</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="19">
         <v>-90</v>
       </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21">
+      <c r="F37" s="19">
+        <v>-12</v>
+      </c>
+      <c r="G37" s="19">
         <v>-150</v>
       </c>
-      <c r="H37" s="21">
+      <c r="H37" s="19">
         <v>-37.5</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="10" customFormat="1">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19">
         <f>SUM(H36:H37)</f>
         <v>2532.4575</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" s="10" customFormat="1">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" s="10" customFormat="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19">
         <v>2532.4575</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" s="10" customFormat="1">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19">
         <v>434.5</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:8" s="10" customFormat="1">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19">
         <v>20</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
     </row>
     <row r="44" spans="1:8" s="10" customFormat="1">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19">
         <f>SUM(B41:B43)</f>
         <v>2986.9575</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
     </row>
     <row r="46" spans="1:8" s="10" customFormat="1">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21" t="s">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19" t="s">
         <v>457</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
     </row>
     <row r="47" spans="1:8" s="10" customFormat="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19">
         <v>4205</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:8" s="10" customFormat="1">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19">
         <v>-90</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
     </row>
     <row r="49" spans="1:8" s="10" customFormat="1">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19">
         <v>-2532.4575</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" s="10" customFormat="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19">
         <v>-434.5</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" s="10" customFormat="1">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19">
         <f>SUM(B47:B50)</f>
         <v>1148.0425</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:8" s="10" customFormat="1">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21" t="s">
+      <c r="A53" s="19"/>
+      <c r="B53" s="19" t="s">
         <v>460</v>
       </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" s="10" customFormat="1">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21">
+      <c r="A54" s="19"/>
+      <c r="B54" s="19">
         <v>1266.2249999999999</v>
       </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" s="10" customFormat="1">
-      <c r="A55" s="21"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21" t="s">
+      <c r="A56" s="19"/>
+      <c r="B56" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21">
+      <c r="A57" s="19"/>
+      <c r="B57" s="19">
         <f>2532.45/2</f>
         <v>1266.2249999999999</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21">
+      <c r="A58" s="19"/>
+      <c r="B58" s="19">
         <v>217.25</v>
       </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="21"/>
-      <c r="B59" s="21">
+      <c r="A59" s="19"/>
+      <c r="B59" s="19">
         <v>12</v>
       </c>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21">
+      <c r="A60" s="19"/>
+      <c r="B60" s="19">
         <v>-440</v>
       </c>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="21"/>
-      <c r="B61" s="21">
+      <c r="A61" s="19"/>
+      <c r="B61" s="19">
         <f>SUM(B57:B60)</f>
         <v>1055.4749999999999</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C61" s="23" t="s">
         <v>461</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="63" spans="1:8">
       <c r="B63" s="10"/>
@@ -3203,13 +3203,13 @@
       <c r="E1" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12">
       <c r="B2">

</xml_diff>